<commit_message>
add models 03 and 04
</commit_message>
<xml_diff>
--- a/data/piloting/scores_slrt.xlsx
+++ b/data/piloting/scores_slrt.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="34">
   <si>
     <t>testperson</t>
   </si>
@@ -123,6 +123,9 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t>biokurs19-09</t>
   </si>
 </sst>
 </file>
@@ -458,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O17"/>
+  <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M14" activeCellId="1" sqref="G14 M14"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -469,7 +472,7 @@
     <col min="2" max="2" width="15.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -513,7 +516,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -557,7 +560,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -601,7 +604,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -645,7 +648,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -689,7 +692,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -733,7 +736,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -777,7 +780,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -821,7 +824,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -865,353 +868,397 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10">
+        <v>137</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>0.73</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>136</v>
+      </c>
+      <c r="G10" s="2">
+        <v>83</v>
+      </c>
+      <c r="H10">
+        <v>102</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>0.98</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>101</v>
+      </c>
+      <c r="M10" s="2">
+        <v>92</v>
+      </c>
+      <c r="N10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>21</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>32</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
         <v>32</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D11" t="s">
         <v>32</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E11" t="s">
         <v>32</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F11" t="s">
         <v>32</v>
       </c>
-      <c r="G10" t="s">
+      <c r="G11" t="s">
         <v>32</v>
       </c>
-      <c r="H10" t="s">
+      <c r="H11" t="s">
         <v>32</v>
       </c>
-      <c r="I10" t="s">
+      <c r="I11" t="s">
         <v>32</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J11" t="s">
         <v>32</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K11" t="s">
         <v>32</v>
       </c>
-      <c r="L10" t="s">
+      <c r="L11" t="s">
         <v>32</v>
       </c>
-      <c r="M10" t="s">
+      <c r="M11" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>22</v>
       </c>
-      <c r="B11">
+      <c r="B12">
         <v>129</v>
       </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
         <v>129</v>
       </c>
-      <c r="G11" s="2">
+      <c r="G12" s="2">
         <v>72.5</v>
       </c>
-      <c r="H11">
+      <c r="H12">
         <v>91</v>
       </c>
-      <c r="I11">
+      <c r="I12">
         <v>2</v>
       </c>
-      <c r="J11">
+      <c r="J12">
         <v>2.2000000000000002</v>
       </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11">
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
         <v>89</v>
       </c>
-      <c r="M11" s="2">
+      <c r="M12" s="2">
         <v>81</v>
       </c>
-      <c r="N11" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+      <c r="N12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>23</v>
       </c>
-      <c r="B12">
+      <c r="B13">
         <v>118</v>
       </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
         <v>118</v>
       </c>
-      <c r="G12" s="2">
+      <c r="G13" s="2">
         <v>40.5</v>
       </c>
-      <c r="H12">
+      <c r="H13">
         <v>64</v>
       </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-      <c r="L12">
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
         <v>64</v>
       </c>
-      <c r="M12" s="2">
+      <c r="M13" s="2">
         <v>25.5</v>
       </c>
-      <c r="N12" t="s">
+      <c r="N13" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>24</v>
       </c>
-      <c r="B13">
+      <c r="B14">
         <v>113</v>
       </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
         <v>113</v>
       </c>
-      <c r="G13" s="2">
+      <c r="G14" s="2">
         <v>44</v>
       </c>
-      <c r="H13">
+      <c r="H14">
         <v>70</v>
       </c>
-      <c r="I13">
+      <c r="I14">
         <v>2</v>
       </c>
-      <c r="J13">
+      <c r="J14">
         <v>5.7</v>
       </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-      <c r="L13">
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
         <v>68</v>
       </c>
-      <c r="M13" s="2">
+      <c r="M14" s="2">
         <v>37.5</v>
       </c>
-      <c r="N13" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A14" s="4" t="s">
+      <c r="N14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A15" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="4">
+      <c r="B15" s="4">
         <v>118</v>
       </c>
-      <c r="C14" s="4">
-        <v>0</v>
-      </c>
-      <c r="D14" s="4">
-        <v>0</v>
-      </c>
-      <c r="E14" s="4">
-        <v>0</v>
-      </c>
-      <c r="F14" s="4">
+      <c r="C15" s="4">
+        <v>0</v>
+      </c>
+      <c r="D15" s="4">
+        <v>0</v>
+      </c>
+      <c r="E15" s="4">
+        <v>0</v>
+      </c>
+      <c r="F15" s="4">
         <v>118</v>
       </c>
-      <c r="G14" s="2">
+      <c r="G15" s="2">
         <v>56.5</v>
       </c>
-      <c r="H14" s="4">
+      <c r="H15" s="4">
         <v>87</v>
       </c>
-      <c r="I14" s="4">
-        <v>0</v>
-      </c>
-      <c r="J14" s="4">
-        <v>0</v>
-      </c>
-      <c r="K14" s="4">
-        <v>0</v>
-      </c>
-      <c r="L14" s="4">
+      <c r="I15" s="4">
+        <v>0</v>
+      </c>
+      <c r="J15" s="4">
+        <v>0</v>
+      </c>
+      <c r="K15" s="4">
+        <v>0</v>
+      </c>
+      <c r="L15" s="4">
         <v>87</v>
       </c>
-      <c r="M14" s="2">
+      <c r="M15" s="2">
         <v>77.5</v>
       </c>
-      <c r="N14" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+      <c r="N15" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
         <v>26</v>
       </c>
-      <c r="B15">
+      <c r="B16">
         <v>134</v>
       </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
         <v>134</v>
       </c>
-      <c r="G15" s="2">
+      <c r="G16" s="2">
         <v>81</v>
       </c>
-      <c r="H15">
+      <c r="H16">
         <v>109</v>
       </c>
-      <c r="I15">
-        <v>0</v>
-      </c>
-      <c r="J15">
-        <v>0</v>
-      </c>
-      <c r="K15">
-        <v>0</v>
-      </c>
-      <c r="L15">
-        <v>0</v>
-      </c>
-      <c r="M15" s="2">
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>109</v>
+      </c>
+      <c r="M16" s="2">
         <v>97.5</v>
       </c>
-      <c r="N15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A16" s="4" t="s">
+      <c r="N16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A17" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B16" s="4">
+      <c r="B17" s="4">
         <v>130</v>
       </c>
-      <c r="C16" s="4">
-        <v>0</v>
-      </c>
-      <c r="D16" s="4">
-        <v>0</v>
-      </c>
-      <c r="E16" s="4">
-        <v>0</v>
-      </c>
-      <c r="F16" s="4">
+      <c r="C17" s="4">
+        <v>0</v>
+      </c>
+      <c r="D17" s="4">
+        <v>0</v>
+      </c>
+      <c r="E17" s="4">
+        <v>0</v>
+      </c>
+      <c r="F17" s="4">
         <v>130</v>
       </c>
-      <c r="G16" s="2">
+      <c r="G17" s="2">
         <v>74</v>
       </c>
-      <c r="H16" s="4">
+      <c r="H17" s="4">
         <v>85</v>
       </c>
-      <c r="I16" s="4">
-        <v>0</v>
-      </c>
-      <c r="J16" s="4">
-        <v>0</v>
-      </c>
-      <c r="K16" s="4">
-        <v>0</v>
-      </c>
-      <c r="L16" s="4">
-        <v>0</v>
-      </c>
-      <c r="M16" s="2">
+      <c r="I17" s="4">
+        <v>0</v>
+      </c>
+      <c r="J17" s="4">
+        <v>0</v>
+      </c>
+      <c r="K17" s="4">
+        <v>0</v>
+      </c>
+      <c r="L17" s="4">
+        <v>85</v>
+      </c>
+      <c r="M17" s="2">
         <v>72.5</v>
       </c>
-      <c r="N16" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="O16" s="4"/>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+      <c r="N17" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="O17" s="4"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
         <v>31</v>
       </c>
-      <c r="B17">
+      <c r="B18">
         <v>118</v>
       </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17">
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
         <v>118</v>
       </c>
-      <c r="G17" s="2">
+      <c r="G18" s="2">
         <v>56.5</v>
       </c>
-      <c r="H17">
+      <c r="H18">
         <v>69</v>
       </c>
-      <c r="I17">
+      <c r="I18">
         <v>1</v>
       </c>
-      <c r="J17">
+      <c r="J18">
         <v>1.45</v>
       </c>
-      <c r="K17">
-        <v>0</v>
-      </c>
-      <c r="L17">
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
         <v>68</v>
       </c>
-      <c r="M17" s="2">
+      <c r="M18" s="2">
         <v>42</v>
       </c>
-      <c r="N17" t="s">
+      <c r="N18" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>